<commit_message>
inter-area mode of 68 bus
</commit_message>
<xml_diff>
--- a/system_cases/Examples/ParticipationAnalysis/ModalConfig_NETS_NYPS_68_modified_detuned.xlsx
+++ b/system_cases/Examples/ParticipationAnalysis/ModalConfig_NETS_NYPS_68_modified_detuned.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRep\Simplus-Grid-Tool\modified_ieee_14\Examples\ParticipationAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRep\Simplus-Grid-Tool\system_cases\Examples\ParticipationAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDA548-53D0-479A-985A-4768C70CAD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2229E494-4698-4728-BA41-AE84A37A1C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4860" yWindow="3970" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{DB46BCEA-93C1-401F-AA84-DD07AA153CA6}"/>
   </bookViews>
@@ -28482,12 +28482,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACAE6F5-0069-4300-89DA-88034066A3FB}">
   <dimension ref="A1:L1240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="A771" workbookViewId="0">
+      <selection activeCell="J790" sqref="J790"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="8" max="8" width="23" customWidth="1"/>
     <col min="11" max="11" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -28570,7 +28571,7 @@
         <v>7</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -28864,7 +28865,7 @@
         <v>523</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -28887,7 +28888,7 @@
         <v>548</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -28956,7 +28957,7 @@
         <v>649</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -37420,7 +37421,7 @@
         <v>1584</v>
       </c>
       <c r="I788">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="789" spans="7:9" x14ac:dyDescent="0.35">
@@ -37442,7 +37443,7 @@
         <v>1588</v>
       </c>
       <c r="I790">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="791" spans="7:9" x14ac:dyDescent="0.35">

</xml_diff>